<commit_message>
chandra manual annot complete
</commit_message>
<xml_diff>
--- a/Chandrashekaran-annotations/AAPL_Q2_2009.xlsx
+++ b/Chandrashekaran-annotations/AAPL_Q2_2009.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vm056257\Downloads\Working\PEBU\ML\SubjECTive-QA\Chandrashekaran-annotations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE7E5D2-097D-4222-98EE-CAD2C19CD9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FDCDAF-977F-491B-9ABD-46FEF73A47AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -639,8 +639,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="88.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,6 +704,24 @@
       <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -717,6 +736,24 @@
       <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="270" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -731,6 +768,24 @@
       <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -745,6 +800,24 @@
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="255" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -759,6 +832,24 @@
       <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -773,6 +864,24 @@
       <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -787,6 +896,24 @@
       <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -801,6 +928,24 @@
       <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -815,6 +960,24 @@
       <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -829,6 +992,24 @@
       <c r="D11" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2</v>
+      </c>
+      <c r="I11" s="2">
+        <v>2</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -843,6 +1024,24 @@
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -857,6 +1056,24 @@
       <c r="D13" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -871,6 +1088,24 @@
       <c r="D14" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="E14" s="2">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -885,6 +1120,24 @@
       <c r="D15" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -899,8 +1152,26 @@
       <c r="D16" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>2</v>
+      </c>
+      <c r="I16" s="2">
+        <v>2</v>
+      </c>
+      <c r="J16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="255" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -913,8 +1184,26 @@
       <c r="D17" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2</v>
+      </c>
+      <c r="G17" s="2">
+        <v>2</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2</v>
+      </c>
+      <c r="I17" s="2">
+        <v>2</v>
+      </c>
+      <c r="J17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -927,8 +1216,26 @@
       <c r="D18" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+      <c r="E18" s="2">
+        <v>2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
+        <v>2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>2</v>
+      </c>
+      <c r="J18" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>47</v>
       </c>
@@ -941,8 +1248,26 @@
       <c r="D19" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E19" s="2">
+        <v>2</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2</v>
+      </c>
+      <c r="I19" s="2">
+        <v>2</v>
+      </c>
+      <c r="J19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
@@ -955,8 +1280,26 @@
       <c r="D20" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>54</v>
       </c>
@@ -969,8 +1312,26 @@
       <c r="D21" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1</v>
+      </c>
+      <c r="J21" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>59</v>
       </c>
@@ -983,8 +1344,26 @@
       <c r="D22" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="345" x14ac:dyDescent="0.25">
+      <c r="E22" s="2">
+        <v>2</v>
+      </c>
+      <c r="F22" s="2">
+        <v>2</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2">
+        <v>2</v>
+      </c>
+      <c r="J22" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="345" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>59</v>
       </c>
@@ -997,8 +1376,26 @@
       <c r="D23" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E23" s="2">
+        <v>2</v>
+      </c>
+      <c r="F23" s="2">
+        <v>2</v>
+      </c>
+      <c r="G23" s="2">
+        <v>2</v>
+      </c>
+      <c r="H23" s="2">
+        <v>2</v>
+      </c>
+      <c r="I23" s="2">
+        <v>2</v>
+      </c>
+      <c r="J23" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>64</v>
       </c>
@@ -1011,8 +1408,26 @@
       <c r="D24" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E24" s="2">
+        <v>2</v>
+      </c>
+      <c r="F24" s="2">
+        <v>2</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>2</v>
+      </c>
+      <c r="I24" s="2">
+        <v>2</v>
+      </c>
+      <c r="J24" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>64</v>
       </c>
@@ -1025,8 +1440,26 @@
       <c r="D25" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="E25" s="2">
+        <v>2</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
+        <v>2</v>
+      </c>
+      <c r="I25" s="2">
+        <v>2</v>
+      </c>
+      <c r="J25" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>69</v>
       </c>
@@ -1039,8 +1472,26 @@
       <c r="D26" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <v>2</v>
+      </c>
+      <c r="J26" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>69</v>
       </c>
@@ -1053,8 +1504,26 @@
       <c r="D27" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2">
+        <v>2</v>
+      </c>
+      <c r="H27" s="2">
+        <v>2</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1</v>
+      </c>
+      <c r="J27" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>69</v>
       </c>
@@ -1067,8 +1536,26 @@
       <c r="D28" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="2">
+        <v>2</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+      <c r="J28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>69</v>
       </c>
@@ -1081,8 +1568,26 @@
       <c r="D29" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+      <c r="E29" s="2">
+        <v>2</v>
+      </c>
+      <c r="F29" s="2">
+        <v>2</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1</v>
+      </c>
+      <c r="J29" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>77</v>
       </c>
@@ -1095,8 +1600,26 @@
       <c r="D30" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E30" s="2">
+        <v>2</v>
+      </c>
+      <c r="F30" s="2">
+        <v>2</v>
+      </c>
+      <c r="G30" s="2">
+        <v>2</v>
+      </c>
+      <c r="H30" s="2">
+        <v>2</v>
+      </c>
+      <c r="I30" s="2">
+        <v>2</v>
+      </c>
+      <c r="J30" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>77</v>
       </c>
@@ -1109,8 +1632,26 @@
       <c r="D31" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E31" s="2">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2">
+        <v>2</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1</v>
+      </c>
+      <c r="I31" s="2">
+        <v>2</v>
+      </c>
+      <c r="J31" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>77</v>
       </c>
@@ -1122,6 +1663,24 @@
       </c>
       <c r="D32" s="2" t="s">
         <v>83</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
+      <c r="F32" s="2">
+        <v>2</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1</v>
+      </c>
+      <c r="H32" s="2">
+        <v>2</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+      <c r="J32" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chandra rows cleaned up count 13
</commit_message>
<xml_diff>
--- a/Chandrashekaran-annotations/AAPL_Q2_2009.xlsx
+++ b/Chandrashekaran-annotations/AAPL_Q2_2009.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vm056257\Downloads\Working\PEBU\ML\SubjECTive-QA\Chandrashekaran-annotations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FDCDAF-977F-491B-9ABD-46FEF73A47AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C8C280-09EB-4D13-890D-F9A7CCF9EABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="82">
   <si>
     <t>Asker</t>
   </si>
@@ -149,12 +149,6 @@
   </si>
   <si>
     <t>On – okay, let me just comment on BRIC in general. We now have of the four BRIC countries, Brazil, Russia, India, and China, we have three of those up and we have 8,000 store counts in those three selling the iPhones and we feel very good about that and we’re putting a lot of energy in growing those. China, we are not in yet. We would like to be in China within the next year and are currently working on that. But I have got nothing specific to announce today on this.</t>
-  </si>
-  <si>
-    <t>Okay. And on Steve Jobs? I will let Peter make a comment there.</t>
-  </si>
-  <si>
-    <t>Gene, what is your question?</t>
   </si>
   <si>
     <t>Any update regarding Steve Jobs and his return?</t>
@@ -637,29 +631,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="88.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="88.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="89.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="88.140625" style="2"/>
+    <col min="10" max="10" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="88.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -691,7 +685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -723,7 +717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -755,7 +749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="270" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -787,7 +781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="288" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -819,7 +813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="255" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -851,7 +845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -883,7 +877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -915,7 +909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -947,7 +941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -979,7 +973,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1011,7 +1005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -1043,7 +1037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -1075,7 +1069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -1107,7 +1101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1121,59 +1115,59 @@
         <v>44</v>
       </c>
       <c r="E15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="2">
         <v>1</v>
       </c>
       <c r="H15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2</v>
+      </c>
+      <c r="H16" s="2">
+        <v>2</v>
+      </c>
+      <c r="I16" s="2">
+        <v>2</v>
+      </c>
+      <c r="J16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="2">
-        <v>2</v>
-      </c>
-      <c r="F16" s="2">
-        <v>2</v>
-      </c>
-      <c r="G16" s="2">
-        <v>1</v>
-      </c>
-      <c r="H16" s="2">
-        <v>2</v>
-      </c>
-      <c r="I16" s="2">
-        <v>2</v>
-      </c>
-      <c r="J16" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="255" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>11</v>
@@ -1191,7 +1185,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17" s="2">
         <v>2</v>
@@ -1203,9 +1197,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>11</v>
@@ -1223,7 +1217,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H18" s="2">
         <v>2</v>
@@ -1235,41 +1229,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="2">
-        <v>2</v>
-      </c>
-      <c r="F19" s="2">
-        <v>2</v>
-      </c>
-      <c r="G19" s="2">
-        <v>2</v>
-      </c>
-      <c r="H19" s="2">
-        <v>2</v>
-      </c>
-      <c r="I19" s="2">
-        <v>2</v>
-      </c>
-      <c r="J19" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>17</v>
@@ -1281,16 +1275,16 @@
         <v>56</v>
       </c>
       <c r="E20" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20" s="2">
         <v>1</v>
@@ -1299,44 +1293,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>2</v>
+      </c>
+      <c r="J21" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="2">
-        <v>2</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2">
-        <v>0</v>
-      </c>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
-      <c r="I21" s="2">
-        <v>1</v>
-      </c>
-      <c r="J21" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="B22" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>60</v>
@@ -1351,10 +1345,10 @@
         <v>2</v>
       </c>
       <c r="G22" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" s="2">
         <v>2</v>
@@ -1363,41 +1357,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="345" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2</v>
+      </c>
+      <c r="F23" s="2">
+        <v>2</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>2</v>
+      </c>
+      <c r="I23" s="2">
+        <v>2</v>
+      </c>
+      <c r="J23" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="2">
-        <v>2</v>
-      </c>
-      <c r="F23" s="2">
-        <v>2</v>
-      </c>
-      <c r="G23" s="2">
-        <v>2</v>
-      </c>
-      <c r="H23" s="2">
-        <v>2</v>
-      </c>
-      <c r="I23" s="2">
-        <v>2</v>
-      </c>
-      <c r="J23" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>17</v>
@@ -1427,44 +1421,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2">
+        <v>2</v>
+      </c>
+      <c r="J25" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="2">
-        <v>2</v>
-      </c>
-      <c r="F25" s="2">
-        <v>2</v>
-      </c>
-      <c r="G25" s="2">
-        <v>1</v>
-      </c>
-      <c r="H25" s="2">
-        <v>2</v>
-      </c>
-      <c r="I25" s="2">
-        <v>2</v>
-      </c>
-      <c r="J25" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>70</v>
@@ -1476,24 +1470,24 @@
         <v>2</v>
       </c>
       <c r="F26" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I26" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J26" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>17</v>
@@ -1511,10 +1505,10 @@
         <v>1</v>
       </c>
       <c r="G27" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I27" s="2">
         <v>1</v>
@@ -1523,73 +1517,73 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+      <c r="J28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2</v>
+      </c>
+      <c r="F29" s="2">
+        <v>2</v>
+      </c>
+      <c r="G29" s="2">
+        <v>2</v>
+      </c>
+      <c r="H29" s="2">
+        <v>2</v>
+      </c>
+      <c r="I29" s="2">
+        <v>2</v>
+      </c>
+      <c r="J29" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="E28" s="2">
-        <v>2</v>
-      </c>
-      <c r="F28" s="2">
-        <v>1</v>
-      </c>
-      <c r="G28" s="2">
-        <v>1</v>
-      </c>
-      <c r="H28" s="2">
-        <v>1</v>
-      </c>
-      <c r="I28" s="2">
-        <v>1</v>
-      </c>
-      <c r="J28" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" s="2">
-        <v>2</v>
-      </c>
-      <c r="F29" s="2">
-        <v>2</v>
-      </c>
-      <c r="G29" s="2">
-        <v>1</v>
-      </c>
-      <c r="H29" s="2">
-        <v>1</v>
-      </c>
-      <c r="I29" s="2">
-        <v>1</v>
-      </c>
-      <c r="J29" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>17</v>
@@ -1607,10 +1601,10 @@
         <v>2</v>
       </c>
       <c r="G30" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H30" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I30" s="2">
         <v>2</v>
@@ -1619,12 +1613,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>80</v>
@@ -1642,44 +1636,12 @@
         <v>1</v>
       </c>
       <c r="H31" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I31" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J31" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="2">
-        <v>2</v>
-      </c>
-      <c r="F32" s="2">
-        <v>2</v>
-      </c>
-      <c r="G32" s="2">
-        <v>1</v>
-      </c>
-      <c r="H32" s="2">
-        <v>2</v>
-      </c>
-      <c r="I32" s="2">
-        <v>1</v>
-      </c>
-      <c r="J32" s="2">
         <v>2</v>
       </c>
     </row>

</xml_diff>